<commit_message>
data contents/excels - new tab
</commit_message>
<xml_diff>
--- a/agents/NDV/NDV-Data-Contents.xlsx
+++ b/agents/NDV/NDV-Data-Contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernanda.dorea\Documents\GitHub\EFSA-disease-profiles\agents\NDV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DiseaseProfiles\agents\NDV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C295CA00-279F-4D48-98FD-2D11BA46F5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC2C8DC-3738-46C0-B887-C47ADD6456B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3780" yWindow="5500" windowWidth="7230" windowHeight="3980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="238">
   <si>
     <t>ID</t>
   </si>
@@ -718,6 +718,24 @@
   </si>
   <si>
     <t>Vaccines-NDV.html</t>
+  </si>
+  <si>
+    <t>The panel to the right summarizes all evidence collected by EFSA from published studies describing natural infections with this agent (as opposed to experimental infections, summarized in the next section). Scroll down through the content.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFSA conducts regular systematic literature reviews covering studies investigating natural infections with this agent, and published in peer-reviewed literature in English since 1970. </t>
+  </si>
+  <si>
+    <t>You can download all data collected through systematic literature review {ref011:here}. Data fields are explained in this {ref012:read-me file}.</t>
+  </si>
+  <si>
+    <t>*The review was last updated in January 2022. The complete list of references is available for download {ref013:here}. If important references to primary studies are missing, contact {ref004:animal-diseases@efsa.europa.eu}. The full review protocol can be downloaded  {ref007:here}.</t>
+  </si>
+  <si>
+    <t>Experimental Inf.</t>
+  </si>
+  <si>
+    <t>Disease-NDV.html</t>
   </si>
 </sst>
 </file>
@@ -733,7 +751,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -743,6 +761,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -759,9 +789,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,15 +1090,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="O98" sqref="O98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1083,7 +1115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1100,7 +1132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1117,7 +1149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1134,7 +1166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1151,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1168,7 +1200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1185,7 +1217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1202,7 +1234,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1219,7 +1251,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1236,7 +1268,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1253,7 +1285,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1270,7 +1302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1287,7 +1319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1304,7 +1336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1321,7 +1353,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1338,7 +1370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1355,7 +1387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1372,437 +1404,437 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
         <v>2</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2">
         <v>2</v>
       </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22">
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>3</v>
+      </c>
+      <c r="B29" s="3">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>5</v>
-      </c>
-      <c r="B23">
+    <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3">
+        <v>4</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>8</v>
+      </c>
+      <c r="B34" s="3">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>9</v>
+      </c>
+      <c r="B35" s="3">
+        <v>3</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>10</v>
+      </c>
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>11</v>
+      </c>
+      <c r="B37" s="3">
+        <v>3</v>
+      </c>
+      <c r="C37" s="3">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>12</v>
+      </c>
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>13</v>
+      </c>
+      <c r="B39" s="3">
+        <v>3</v>
+      </c>
+      <c r="C39" s="3">
+        <v>5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>14</v>
+      </c>
+      <c r="B40" s="3">
+        <v>3</v>
+      </c>
+      <c r="C40" s="3">
         <v>2</v>
       </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6</v>
-      </c>
-      <c r="B24">
+      <c r="D40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>15</v>
+      </c>
+      <c r="B41" s="3">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3">
+        <v>3</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>16</v>
+      </c>
+      <c r="B42" s="3">
+        <v>3</v>
+      </c>
+      <c r="C42" s="3">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>2</v>
       </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>7</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>8</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>10</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>11</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>12</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>13</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>14</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>15</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>17</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>3</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>4</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>5</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>6</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-      <c r="D41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>7</v>
-      </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>8</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-      <c r="D43" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>9</v>
-      </c>
       <c r="B44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -1811,607 +1843,607 @@
         <v>11</v>
       </c>
       <c r="E44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>10</v>
       </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45">
-        <v>3</v>
-      </c>
-      <c r="D45" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>11</v>
       </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46">
-        <v>3</v>
-      </c>
-      <c r="D46" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>11</v>
       </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="C47">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
         <v>16</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E54" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>12</v>
       </c>
-      <c r="B48">
-        <v>3</v>
-      </c>
-      <c r="C48">
-        <v>4</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
         <v>16</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E55" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>13</v>
-      </c>
-      <c r="B49">
-        <v>3</v>
-      </c>
-      <c r="C49">
-        <v>4</v>
-      </c>
-      <c r="D49" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>13</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
         <v>16</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E56" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>14</v>
       </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
         <v>24</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E57" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>15</v>
       </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="C51">
-        <v>5</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
         <v>24</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E58" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
         <v>16</v>
       </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
-      <c r="C52">
-        <v>5</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
         <v>24</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E59" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>17</v>
       </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
-      <c r="C53">
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60">
         <v>10</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D60" t="s">
         <v>45</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E60" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
         <v>9</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E61" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>2</v>
       </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55">
-        <v>3</v>
-      </c>
-      <c r="D55" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>3</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
-      <c r="D56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>4</v>
-      </c>
-      <c r="B57">
-        <v>4</v>
-      </c>
-      <c r="C57">
-        <v>3</v>
-      </c>
-      <c r="D57" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>5</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>5</v>
-      </c>
-      <c r="B58">
-        <v>4</v>
-      </c>
-      <c r="C58">
-        <v>4</v>
-      </c>
-      <c r="D58" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
         <v>16</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E65" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>6</v>
       </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59">
-        <v>4</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
         <v>16</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E66" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
         <v>7</v>
       </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60">
-        <v>4</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
         <v>16</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E67" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>8</v>
       </c>
-      <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="C61">
-        <v>4</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
         <v>16</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E68" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
         <v>9</v>
       </c>
-      <c r="B62">
-        <v>4</v>
-      </c>
-      <c r="C62">
-        <v>5</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
         <v>24</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E69" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>10</v>
       </c>
-      <c r="B63">
-        <v>4</v>
-      </c>
-      <c r="C63">
-        <v>5</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70" t="s">
         <v>24</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
         <v>11</v>
       </c>
-      <c r="B64">
-        <v>4</v>
-      </c>
-      <c r="C64">
-        <v>5</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71" t="s">
         <v>24</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E71" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
         <v>12</v>
       </c>
-      <c r="B65">
-        <v>4</v>
-      </c>
-      <c r="C65">
+      <c r="B72">
+        <v>5</v>
+      </c>
+      <c r="C72">
         <v>10</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D72" t="s">
         <v>45</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>1</v>
-      </c>
-      <c r="B66">
-        <v>5</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-      <c r="D66" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
         <v>9</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
         <v>2</v>
       </c>
-      <c r="B67">
-        <v>5</v>
-      </c>
-      <c r="C67">
-        <v>3</v>
-      </c>
-      <c r="D67" t="s">
-        <v>13</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="B74">
+        <v>6</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>3</v>
-      </c>
-      <c r="B68">
-        <v>5</v>
-      </c>
-      <c r="C68">
-        <v>3</v>
-      </c>
-      <c r="D68" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>6</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>4</v>
-      </c>
-      <c r="B69">
-        <v>5</v>
-      </c>
-      <c r="C69">
-        <v>3</v>
-      </c>
-      <c r="D69" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>4</v>
+      </c>
+      <c r="B76">
+        <v>6</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>5</v>
-      </c>
-      <c r="B70">
-        <v>5</v>
-      </c>
-      <c r="C70">
-        <v>3</v>
-      </c>
-      <c r="D70" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>6</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
         <v>6</v>
-      </c>
-      <c r="B71">
-        <v>5</v>
-      </c>
-      <c r="C71">
-        <v>4</v>
-      </c>
-      <c r="D71" t="s">
-        <v>16</v>
-      </c>
-      <c r="E71" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>7</v>
-      </c>
-      <c r="B72">
-        <v>5</v>
-      </c>
-      <c r="C72">
-        <v>4</v>
-      </c>
-      <c r="D72" t="s">
-        <v>16</v>
-      </c>
-      <c r="E72" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>8</v>
-      </c>
-      <c r="B73">
-        <v>5</v>
-      </c>
-      <c r="C73">
-        <v>3</v>
-      </c>
-      <c r="D73" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>9</v>
-      </c>
-      <c r="B74">
-        <v>5</v>
-      </c>
-      <c r="C74">
-        <v>3</v>
-      </c>
-      <c r="D74" t="s">
-        <v>13</v>
-      </c>
-      <c r="E74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>10</v>
-      </c>
-      <c r="B75">
-        <v>5</v>
-      </c>
-      <c r="C75">
-        <v>5</v>
-      </c>
-      <c r="D75" t="s">
-        <v>24</v>
-      </c>
-      <c r="E75" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>11</v>
-      </c>
-      <c r="B76">
-        <v>5</v>
-      </c>
-      <c r="C76">
-        <v>5</v>
-      </c>
-      <c r="D76" t="s">
-        <v>24</v>
-      </c>
-      <c r="E76" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>12</v>
-      </c>
-      <c r="B77">
-        <v>5</v>
-      </c>
-      <c r="C77">
-        <v>10</v>
-      </c>
-      <c r="D77" t="s">
-        <v>45</v>
-      </c>
-      <c r="E77" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>1</v>
       </c>
       <c r="B78">
         <v>6</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E78" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B79">
         <v>6</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B80">
         <v>6</v>
@@ -2423,12 +2455,12 @@
         <v>13</v>
       </c>
       <c r="E80" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B81">
         <v>6</v>
@@ -2440,406 +2472,406 @@
         <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B82">
         <v>6</v>
       </c>
-      <c r="C82" s="1">
-        <v>3</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>24</v>
+      </c>
+      <c r="E82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B83">
         <v>6</v>
       </c>
-      <c r="C83" s="1">
-        <v>3</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B84">
         <v>6</v>
       </c>
-      <c r="C84" s="1">
-        <v>3</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E84" s="1" t="s">
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>7</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2</v>
+      </c>
+      <c r="B86">
+        <v>7</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>7</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>4</v>
+      </c>
+      <c r="B88">
+        <v>7</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>13</v>
+      </c>
+      <c r="E88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>7</v>
+      </c>
+      <c r="C89" s="1">
+        <v>3</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>6</v>
+      </c>
+      <c r="B90">
+        <v>7</v>
+      </c>
+      <c r="C90" s="1">
+        <v>3</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>7</v>
+      </c>
+      <c r="B91">
+        <v>7</v>
+      </c>
+      <c r="C91" s="1">
+        <v>3</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="92" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92">
         <v>8</v>
-      </c>
-      <c r="B85">
-        <v>6</v>
-      </c>
-      <c r="C85" s="1">
-        <v>4</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>9</v>
-      </c>
-      <c r="B86">
-        <v>6</v>
-      </c>
-      <c r="C86" s="1">
-        <v>4</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>10</v>
-      </c>
-      <c r="B87">
-        <v>6</v>
-      </c>
-      <c r="C87" s="1">
-        <v>3</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>11</v>
-      </c>
-      <c r="B88">
-        <v>6</v>
-      </c>
-      <c r="C88" s="1">
-        <v>3</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>12</v>
-      </c>
-      <c r="B89">
-        <v>6</v>
-      </c>
-      <c r="C89" s="1">
-        <v>5</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>13</v>
-      </c>
-      <c r="B90">
-        <v>6</v>
-      </c>
-      <c r="C90" s="1">
-        <v>5</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>14</v>
-      </c>
-      <c r="B91">
-        <v>6</v>
-      </c>
-      <c r="C91" s="1">
-        <v>10</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>1</v>
       </c>
       <c r="B92">
         <v>7</v>
       </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="C92" s="1">
+        <v>4</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93">
         <v>9</v>
-      </c>
-      <c r="E92" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>2</v>
       </c>
       <c r="B93">
         <v>7</v>
       </c>
-      <c r="C93">
-        <v>3</v>
-      </c>
-      <c r="D93" t="s">
-        <v>13</v>
-      </c>
-      <c r="E93" t="s">
+      <c r="C93" s="1">
+        <v>4</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>10</v>
+      </c>
+      <c r="B94">
+        <v>7</v>
+      </c>
+      <c r="C94" s="1">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>11</v>
+      </c>
+      <c r="B95">
+        <v>7</v>
+      </c>
+      <c r="C95" s="1">
+        <v>3</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>12</v>
+      </c>
+      <c r="B96">
+        <v>7</v>
+      </c>
+      <c r="C96" s="1">
+        <v>5</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>13</v>
+      </c>
+      <c r="B97">
+        <v>7</v>
+      </c>
+      <c r="C97" s="1">
+        <v>5</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>14</v>
+      </c>
+      <c r="B98">
+        <v>7</v>
+      </c>
+      <c r="C98" s="1">
+        <v>10</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="B99">
+        <v>8</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100">
+        <v>8</v>
+      </c>
+      <c r="C100">
+        <v>3</v>
+      </c>
+      <c r="D100" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>1</v>
-      </c>
-      <c r="B94">
-        <v>8</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="D94" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>2</v>
-      </c>
-      <c r="B95">
-        <v>8</v>
-      </c>
-      <c r="C95">
-        <v>3</v>
-      </c>
-      <c r="D95" t="s">
-        <v>13</v>
-      </c>
-      <c r="E95" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>3</v>
-      </c>
-      <c r="B96">
-        <v>8</v>
-      </c>
-      <c r="C96">
-        <v>3</v>
-      </c>
-      <c r="D96" t="s">
-        <v>13</v>
-      </c>
-      <c r="E96" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>4</v>
-      </c>
-      <c r="B97">
-        <v>8</v>
-      </c>
-      <c r="C97">
-        <v>10</v>
-      </c>
-      <c r="D97" t="s">
-        <v>45</v>
-      </c>
-      <c r="E97" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>1</v>
-      </c>
-      <c r="B98">
-        <v>9</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="D98" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>2</v>
-      </c>
-      <c r="B99">
-        <v>9</v>
-      </c>
-      <c r="C99">
-        <v>3</v>
-      </c>
-      <c r="D99" t="s">
-        <v>13</v>
-      </c>
-      <c r="E99" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>3</v>
-      </c>
-      <c r="B100">
-        <v>9</v>
-      </c>
-      <c r="C100">
-        <v>3</v>
-      </c>
-      <c r="D100" t="s">
-        <v>13</v>
-      </c>
-      <c r="E100" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B101">
         <v>9</v>
       </c>
       <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>9</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
+      </c>
+      <c r="D102" t="s">
+        <v>13</v>
+      </c>
+      <c r="E102" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <v>9</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
+        <v>13</v>
+      </c>
+      <c r="E103" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>9</v>
+      </c>
+      <c r="C104">
         <v>10</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D104" t="s">
         <v>45</v>
       </c>
-      <c r="E101" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>1</v>
-      </c>
-      <c r="B102">
+      <c r="E104" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
         <v>10</v>
-      </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-      <c r="D102" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>2</v>
-      </c>
-      <c r="B103">
-        <v>10</v>
-      </c>
-      <c r="C103">
-        <v>3</v>
-      </c>
-      <c r="D103" t="s">
-        <v>13</v>
-      </c>
-      <c r="E103" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>3</v>
-      </c>
-      <c r="B104">
-        <v>10</v>
-      </c>
-      <c r="C104">
-        <v>13</v>
-      </c>
-      <c r="D104" t="s">
-        <v>99</v>
-      </c>
-      <c r="E104" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>1</v>
-      </c>
-      <c r="B105">
-        <v>11</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -2848,15 +2880,15 @@
         <v>9</v>
       </c>
       <c r="E105" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2</v>
       </c>
       <c r="B106">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -2865,15 +2897,15 @@
         <v>13</v>
       </c>
       <c r="E106" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>3</v>
       </c>
       <c r="B107">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -2882,78 +2914,78 @@
         <v>13</v>
       </c>
       <c r="E107" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>4</v>
       </c>
       <c r="B108">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C108">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D108" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="E108" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B109">
         <v>11</v>
       </c>
       <c r="C109">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E109" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B110">
         <v>11</v>
       </c>
       <c r="C110">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D110" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E110" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B111">
         <v>11</v>
       </c>
       <c r="C111">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D111" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E111" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>1</v>
       </c>
@@ -2967,10 +2999,10 @@
         <v>9</v>
       </c>
       <c r="E112" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2</v>
       </c>
@@ -2984,10 +3016,10 @@
         <v>13</v>
       </c>
       <c r="E113" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>3</v>
       </c>
@@ -3001,10 +3033,10 @@
         <v>13</v>
       </c>
       <c r="E114" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>4</v>
       </c>
@@ -3012,16 +3044,16 @@
         <v>12</v>
       </c>
       <c r="C115">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D115" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E115" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>5</v>
       </c>
@@ -3035,10 +3067,10 @@
         <v>16</v>
       </c>
       <c r="E116" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>6</v>
       </c>
@@ -3052,10 +3084,10 @@
         <v>16</v>
       </c>
       <c r="E117" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>7</v>
       </c>
@@ -3063,63 +3095,182 @@
         <v>12</v>
       </c>
       <c r="C118">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D118" t="s">
+        <v>107</v>
+      </c>
+      <c r="E118" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>13</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120">
+        <v>13</v>
+      </c>
+      <c r="C120">
+        <v>3</v>
+      </c>
+      <c r="D120" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>3</v>
+      </c>
+      <c r="B121">
+        <v>13</v>
+      </c>
+      <c r="C121">
+        <v>3</v>
+      </c>
+      <c r="D121" t="s">
+        <v>13</v>
+      </c>
+      <c r="E121" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>4</v>
+      </c>
+      <c r="B122">
+        <v>13</v>
+      </c>
+      <c r="C122">
+        <v>4</v>
+      </c>
+      <c r="D122" t="s">
         <v>16</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E122" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>5</v>
+      </c>
+      <c r="B123">
+        <v>13</v>
+      </c>
+      <c r="C123">
+        <v>4</v>
+      </c>
+      <c r="D123" t="s">
+        <v>16</v>
+      </c>
+      <c r="E123" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>6</v>
+      </c>
+      <c r="B124">
+        <v>13</v>
+      </c>
+      <c r="C124">
+        <v>4</v>
+      </c>
+      <c r="D124" t="s">
+        <v>16</v>
+      </c>
+      <c r="E124" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>7</v>
+      </c>
+      <c r="B125">
+        <v>13</v>
+      </c>
+      <c r="C125">
+        <v>4</v>
+      </c>
+      <c r="D125" t="s">
+        <v>16</v>
+      </c>
+      <c r="E125" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126">
         <v>8</v>
       </c>
-      <c r="B119">
-        <v>12</v>
-      </c>
-      <c r="C119">
-        <v>4</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="B126">
+        <v>13</v>
+      </c>
+      <c r="C126">
+        <v>4</v>
+      </c>
+      <c r="D126" t="s">
         <v>16</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E126" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127">
         <v>9</v>
       </c>
-      <c r="B120">
-        <v>12</v>
-      </c>
-      <c r="C120">
-        <v>4</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="B127">
+        <v>13</v>
+      </c>
+      <c r="C127">
+        <v>4</v>
+      </c>
+      <c r="D127" t="s">
         <v>16</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E127" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128">
         <v>10</v>
       </c>
-      <c r="B121">
-        <v>12</v>
-      </c>
-      <c r="C121">
-        <v>4</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="B128">
+        <v>13</v>
+      </c>
+      <c r="C128">
+        <v>4</v>
+      </c>
+      <c r="D128" t="s">
         <v>16</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E128" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3135,9 +3286,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3151,7 +3302,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3165,7 +3316,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3179,7 +3330,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -3193,7 +3344,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -3207,7 +3358,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3221,7 +3372,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -3235,7 +3386,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -3249,7 +3400,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -3263,7 +3414,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -3277,7 +3428,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -3291,7 +3442,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -3305,7 +3456,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -3319,7 +3470,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -3333,7 +3484,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>161</v>
       </c>
@@ -3347,7 +3498,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -3361,7 +3512,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -3375,7 +3526,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>170</v>
       </c>
@@ -3389,7 +3540,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>173</v>
       </c>
@@ -3403,7 +3554,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>176</v>
       </c>
@@ -3417,7 +3568,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>179</v>
       </c>
@@ -3431,7 +3582,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -3445,7 +3596,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -3459,7 +3610,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>188</v>
       </c>
@@ -3473,7 +3624,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>191</v>
       </c>
@@ -3487,7 +3638,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>194</v>
       </c>
@@ -3501,7 +3652,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>197</v>
       </c>
@@ -3515,7 +3666,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>200</v>
       </c>
@@ -3529,7 +3680,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>203</v>
       </c>
@@ -3543,7 +3694,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>206</v>
       </c>
@@ -3557,7 +3708,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -3571,7 +3722,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>212</v>
       </c>
@@ -3585,7 +3736,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -3599,7 +3750,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>218</v>
       </c>
@@ -3613,7 +3764,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>221</v>
       </c>

</xml_diff>